<commit_message>
I added nwe data
</commit_message>
<xml_diff>
--- a/Companies_transpose_edited_2_final.xlsx
+++ b/Companies_transpose_edited_2_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Data\Thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF56052D-8F53-405A-950E-9CC2D6815959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767A51F7-1FA7-431B-AA81-190FE8060D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1042,7 +1042,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1050,11 +1050,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1359,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AZ643"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q43" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AN88" sqref="AN88"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AZ15" sqref="AZ15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -94727,7 +94726,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726E759D-8BB9-4D74-938C-309E662FF30B}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="P1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="A1:K14"/>
@@ -94735,8 +94734,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5" customWidth="1"/>
-    <col min="2" max="15" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="16" max="17" width="9.140625" style="4"/>
   </cols>
   <sheetData/>

</xml_diff>